<commit_message>
pilot version, changed name to CRLh and CRLe
</commit_message>
<xml_diff>
--- a/design/sets.xlsx
+++ b/design/sets.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/santiago_castiellodeobeso_yale_edu/Documents/Collaborations/Brooklyn_College/categoricalReversalLerning/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E648701-6A66-4FB2-9BE9-5E17CB58D7AF}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D3FDCAC-F565-494C-B6AE-99B71A65B74B}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="33">
   <si>
     <t>phase</t>
   </si>
@@ -112,6 +123,18 @@
   </si>
   <si>
     <t>Easy</t>
+  </si>
+  <si>
+    <t>Set5</t>
+  </si>
+  <si>
+    <t>Set6</t>
+  </si>
+  <si>
+    <t>Set7</t>
+  </si>
+  <si>
+    <t>Set8</t>
   </si>
 </sst>
 </file>
@@ -218,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,11 +287,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,8 +296,14 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y52"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="79" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="E48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T69" sqref="T69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -594,80 +620,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="29" t="s">
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="30" t="s">
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
     </row>
     <row r="2" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28" t="s">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29" t="s">
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29" t="s">
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="30" t="s">
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30" t="s">
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="14" t="s">
@@ -744,7 +770,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="27" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="26">
@@ -821,7 +847,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="31"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="26">
         <v>1</v>
       </c>
@@ -896,7 +922,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="31"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="26">
         <v>1</v>
       </c>
@@ -971,7 +997,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="31"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="26">
         <v>1</v>
       </c>
@@ -1046,7 +1072,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="31"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="26">
         <v>1</v>
       </c>
@@ -1121,7 +1147,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="31"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="26">
         <v>1</v>
       </c>
@@ -1196,7 +1222,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="31"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="26">
         <v>1</v>
       </c>
@@ -1271,7 +1297,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="31"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="26">
         <v>1</v>
       </c>
@@ -1346,7 +1372,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="31"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="26">
         <v>1</v>
       </c>
@@ -1421,7 +1447,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="31"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="26">
         <v>1</v>
       </c>
@@ -1496,7 +1522,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="31"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="26">
         <v>1</v>
       </c>
@@ -1571,7 +1597,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="31"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="26">
         <v>1</v>
       </c>
@@ -1646,7 +1672,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="31"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="26">
         <v>1</v>
       </c>
@@ -1721,7 +1747,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="31"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="26">
         <v>1</v>
       </c>
@@ -1796,7 +1822,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="31"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="26">
         <v>1</v>
       </c>
@@ -1871,7 +1897,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="31"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="26">
         <v>1</v>
       </c>
@@ -1946,7 +1972,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="31"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="14">
         <v>2</v>
       </c>
@@ -2021,7 +2047,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="31"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="14">
         <v>2</v>
       </c>
@@ -2096,7 +2122,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="31"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="14">
         <v>2</v>
       </c>
@@ -2171,7 +2197,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="31"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="14">
         <v>2</v>
       </c>
@@ -2246,7 +2272,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="31"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="14">
         <v>2</v>
       </c>
@@ -2321,7 +2347,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="31"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="14">
         <v>2</v>
       </c>
@@ -2396,7 +2422,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="31"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="14">
         <v>2</v>
       </c>
@@ -2471,7 +2497,7 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="31"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="14">
         <v>2</v>
       </c>
@@ -2546,7 +2572,7 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="31"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="14">
         <v>2</v>
       </c>
@@ -2621,7 +2647,7 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="31"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="14">
         <v>2</v>
       </c>
@@ -2696,7 +2722,7 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="31"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="14">
         <v>2</v>
       </c>
@@ -2771,7 +2797,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="31"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="14">
         <v>2</v>
       </c>
@@ -2846,7 +2872,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="31"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -2921,7 +2947,7 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="31"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="14">
         <v>2</v>
       </c>
@@ -2996,7 +3022,7 @@
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="31"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -3071,7 +3097,7 @@
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="31"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="14">
         <v>2</v>
       </c>
@@ -3146,25 +3172,41 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="Y36"/>
+      <c r="B36" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="26">
@@ -3189,35 +3231,35 @@
         <v>1</v>
       </c>
       <c r="I37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+      <c r="L37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J37" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" s="1">
-        <v>1</v>
-      </c>
-      <c r="L37" s="2" t="s">
+      <c r="M37" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N37" s="3">
+        <v>1</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P37" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>1</v>
+      </c>
+      <c r="R37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M37" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="N37" s="3">
-        <v>1</v>
-      </c>
-      <c r="O37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P37" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q37" s="3">
-        <v>1</v>
-      </c>
-      <c r="R37" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="S37" s="23" t="s">
         <v>4</v>
       </c>
@@ -3225,7 +3267,7 @@
         <v>1</v>
       </c>
       <c r="U37" s="7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="V37" s="25" t="s">
         <v>4</v>
@@ -3234,14 +3276,14 @@
         <v>1</v>
       </c>
       <c r="X37" s="7" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="Y37" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="31"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="26">
         <v>1</v>
       </c>
@@ -3264,35 +3306,35 @@
         <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="1">
+        <v>1</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J38" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="1">
-        <v>1</v>
-      </c>
-      <c r="L38" s="2" t="s">
+      <c r="M38" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N38" s="3">
+        <v>1</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P38" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>1</v>
+      </c>
+      <c r="R38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M38" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="N38" s="3">
-        <v>1</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P38" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q38" s="3">
-        <v>1</v>
-      </c>
-      <c r="R38" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="S38" s="23" t="s">
         <v>4</v>
       </c>
@@ -3300,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="U38" s="7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="V38" s="25" t="s">
         <v>4</v>
@@ -3309,14 +3351,14 @@
         <v>1</v>
       </c>
       <c r="X38" s="7" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="Y38" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="31"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="26">
         <v>1</v>
       </c>
@@ -3339,35 +3381,35 @@
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="1">
+        <v>1</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="K39" s="1">
-        <v>1</v>
-      </c>
-      <c r="L39" s="2" t="s">
+      <c r="M39" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N39" s="3">
+        <v>1</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P39" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>1</v>
+      </c>
+      <c r="R39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M39" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="N39" s="3">
-        <v>1</v>
-      </c>
-      <c r="O39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q39" s="3">
-        <v>1</v>
-      </c>
-      <c r="R39" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="S39" s="23" t="s">
         <v>4</v>
       </c>
@@ -3375,23 +3417,23 @@
         <v>1</v>
       </c>
       <c r="U39" s="7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V39" s="25" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="W39" s="6">
         <v>1</v>
       </c>
       <c r="X39" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="Y39" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="31"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="26">
         <v>1</v>
       </c>
@@ -3414,35 +3456,35 @@
         <v>1</v>
       </c>
       <c r="I40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J40" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="K40" s="1">
-        <v>1</v>
-      </c>
-      <c r="L40" s="2" t="s">
+      <c r="M40" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N40" s="3">
+        <v>1</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P40" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>1</v>
+      </c>
+      <c r="R40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M40" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="N40" s="3">
-        <v>1</v>
-      </c>
-      <c r="O40" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P40" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q40" s="3">
-        <v>1</v>
-      </c>
-      <c r="R40" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="S40" s="23" t="s">
         <v>4</v>
       </c>
@@ -3450,23 +3492,23 @@
         <v>1</v>
       </c>
       <c r="U40" s="7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V40" s="25" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="W40" s="6">
         <v>1</v>
       </c>
       <c r="X40" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="Y40" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="31"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="26">
         <v>1</v>
       </c>
@@ -3489,35 +3531,35 @@
         <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K41" s="1">
+        <v>1</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J41" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K41" s="1">
-        <v>1</v>
-      </c>
-      <c r="L41" s="2" t="s">
+      <c r="M41" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N41" s="3">
+        <v>1</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P41" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>1</v>
+      </c>
+      <c r="R41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M41" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="N41" s="3">
-        <v>1</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P41" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q41" s="3">
-        <v>1</v>
-      </c>
-      <c r="R41" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="S41" s="23" t="s">
         <v>9</v>
       </c>
@@ -3525,23 +3567,23 @@
         <v>1</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="V41" s="25" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W41" s="6">
         <v>1</v>
       </c>
       <c r="X41" s="7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y41" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="31"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="26">
         <v>1</v>
       </c>
@@ -3564,35 +3606,35 @@
         <v>1</v>
       </c>
       <c r="I42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K42" s="1">
+        <v>1</v>
+      </c>
+      <c r="L42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J42" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K42" s="1">
-        <v>1</v>
-      </c>
-      <c r="L42" s="2" t="s">
+      <c r="M42" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" s="3">
+        <v>1</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P42" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>1</v>
+      </c>
+      <c r="R42" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M42" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="N42" s="3">
-        <v>1</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P42" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q42" s="3">
-        <v>1</v>
-      </c>
-      <c r="R42" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="S42" s="23" t="s">
         <v>9</v>
       </c>
@@ -3600,23 +3642,23 @@
         <v>1</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="V42" s="25" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W42" s="6">
         <v>1</v>
       </c>
       <c r="X42" s="7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y42" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="31"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="26">
         <v>1</v>
       </c>
@@ -3639,35 +3681,35 @@
         <v>1</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K43" s="1">
+        <v>1</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J43" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="K43" s="1">
-        <v>1</v>
-      </c>
-      <c r="L43" s="2" t="s">
+      <c r="M43" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N43" s="3">
+        <v>1</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P43" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>1</v>
+      </c>
+      <c r="R43" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M43" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="N43" s="3">
-        <v>1</v>
-      </c>
-      <c r="O43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P43" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q43" s="3">
-        <v>1</v>
-      </c>
-      <c r="R43" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="S43" s="23" t="s">
         <v>9</v>
       </c>
@@ -3675,7 +3717,7 @@
         <v>1</v>
       </c>
       <c r="U43" s="7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="V43" s="25" t="s">
         <v>9</v>
@@ -3684,14 +3726,14 @@
         <v>1</v>
       </c>
       <c r="X43" s="7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y43" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="31"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="26">
         <v>1</v>
       </c>
@@ -3714,35 +3756,35 @@
         <v>1</v>
       </c>
       <c r="I44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J44" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="K44" s="1">
-        <v>1</v>
-      </c>
-      <c r="L44" s="2" t="s">
+      <c r="M44" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N44" s="3">
+        <v>1</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P44" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>1</v>
+      </c>
+      <c r="R44" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M44" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="N44" s="3">
-        <v>1</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P44" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q44" s="3">
-        <v>1</v>
-      </c>
-      <c r="R44" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="S44" s="23" t="s">
         <v>9</v>
       </c>
@@ -3750,7 +3792,7 @@
         <v>1</v>
       </c>
       <c r="U44" s="7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="V44" s="25" t="s">
         <v>9</v>
@@ -3759,14 +3801,14 @@
         <v>1</v>
       </c>
       <c r="X44" s="7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y44" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="31"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="14">
         <v>2</v>
       </c>
@@ -3789,35 +3831,35 @@
         <v>2</v>
       </c>
       <c r="I45" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" s="12">
+        <v>2</v>
+      </c>
+      <c r="L45" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J45" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K45" s="12">
-        <v>2</v>
-      </c>
-      <c r="L45" s="13" t="s">
+      <c r="M45" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N45" s="10">
+        <v>2</v>
+      </c>
+      <c r="O45" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P45" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q45" s="10">
+        <v>2</v>
+      </c>
+      <c r="R45" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M45" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="N45" s="10">
-        <v>2</v>
-      </c>
-      <c r="O45" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="P45" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q45" s="10">
-        <v>2</v>
-      </c>
-      <c r="R45" s="11" t="s">
-        <v>8</v>
-      </c>
       <c r="S45" s="22" t="s">
         <v>4</v>
       </c>
@@ -3825,7 +3867,7 @@
         <v>2</v>
       </c>
       <c r="U45" s="9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="V45" s="24" t="s">
         <v>9</v>
@@ -3834,14 +3876,14 @@
         <v>2</v>
       </c>
       <c r="X45" s="9" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="Y45" s="24" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="31"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="14">
         <v>2</v>
       </c>
@@ -3864,35 +3906,35 @@
         <v>2</v>
       </c>
       <c r="I46" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="12">
+        <v>2</v>
+      </c>
+      <c r="L46" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K46" s="12">
-        <v>2</v>
-      </c>
-      <c r="L46" s="13" t="s">
+      <c r="M46" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N46" s="10">
+        <v>2</v>
+      </c>
+      <c r="O46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P46" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q46" s="10">
+        <v>2</v>
+      </c>
+      <c r="R46" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M46" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="N46" s="10">
-        <v>2</v>
-      </c>
-      <c r="O46" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="P46" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q46" s="10">
-        <v>2</v>
-      </c>
-      <c r="R46" s="11" t="s">
-        <v>8</v>
-      </c>
       <c r="S46" s="22" t="s">
         <v>4</v>
       </c>
@@ -3900,7 +3942,7 @@
         <v>2</v>
       </c>
       <c r="U46" s="9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="V46" s="24" t="s">
         <v>9</v>
@@ -3909,14 +3951,14 @@
         <v>2</v>
       </c>
       <c r="X46" s="9" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="Y46" s="24" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="31"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="14">
         <v>2</v>
       </c>
@@ -3939,35 +3981,35 @@
         <v>2</v>
       </c>
       <c r="I47" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="12">
+        <v>2</v>
+      </c>
+      <c r="L47" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J47" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K47" s="12">
-        <v>2</v>
-      </c>
-      <c r="L47" s="13" t="s">
+      <c r="M47" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N47" s="10">
+        <v>2</v>
+      </c>
+      <c r="O47" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P47" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q47" s="10">
+        <v>2</v>
+      </c>
+      <c r="R47" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M47" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N47" s="10">
-        <v>2</v>
-      </c>
-      <c r="O47" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P47" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q47" s="10">
-        <v>2</v>
-      </c>
-      <c r="R47" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="S47" s="22" t="s">
         <v>9</v>
       </c>
@@ -3975,23 +4017,23 @@
         <v>2</v>
       </c>
       <c r="U47" s="9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V47" s="24" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W47" s="8">
         <v>2</v>
       </c>
       <c r="X47" s="9" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="Y47" s="24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="31"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="14">
         <v>2</v>
       </c>
@@ -4014,35 +4056,35 @@
         <v>2</v>
       </c>
       <c r="I48" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="12">
+        <v>2</v>
+      </c>
+      <c r="L48" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J48" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K48" s="12">
-        <v>2</v>
-      </c>
-      <c r="L48" s="13" t="s">
+      <c r="M48" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N48" s="10">
+        <v>2</v>
+      </c>
+      <c r="O48" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P48" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q48" s="10">
+        <v>2</v>
+      </c>
+      <c r="R48" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M48" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N48" s="10">
-        <v>2</v>
-      </c>
-      <c r="O48" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P48" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q48" s="10">
-        <v>2</v>
-      </c>
-      <c r="R48" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="S48" s="22" t="s">
         <v>9</v>
       </c>
@@ -4050,23 +4092,23 @@
         <v>2</v>
       </c>
       <c r="U48" s="9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V48" s="24" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W48" s="8">
         <v>2</v>
       </c>
       <c r="X48" s="9" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="Y48" s="24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="31"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="14">
         <v>2</v>
       </c>
@@ -4089,35 +4131,35 @@
         <v>2</v>
       </c>
       <c r="I49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J49" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K49" s="12">
+        <v>2</v>
+      </c>
+      <c r="L49" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J49" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K49" s="12">
-        <v>2</v>
-      </c>
-      <c r="L49" s="13" t="s">
+      <c r="M49" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N49" s="10">
+        <v>2</v>
+      </c>
+      <c r="O49" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P49" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q49" s="10">
+        <v>2</v>
+      </c>
+      <c r="R49" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M49" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N49" s="10">
-        <v>2</v>
-      </c>
-      <c r="O49" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P49" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q49" s="10">
-        <v>2</v>
-      </c>
-      <c r="R49" s="11" t="s">
-        <v>11</v>
-      </c>
       <c r="S49" s="22" t="s">
         <v>9</v>
       </c>
@@ -4125,23 +4167,23 @@
         <v>2</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="V49" s="24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="W49" s="8">
         <v>2</v>
       </c>
       <c r="X49" s="9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y49" s="24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="31"/>
+      <c r="A50" s="27"/>
       <c r="B50" s="14">
         <v>2</v>
       </c>
@@ -4164,35 +4206,35 @@
         <v>2</v>
       </c>
       <c r="I50" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K50" s="12">
+        <v>2</v>
+      </c>
+      <c r="L50" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J50" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K50" s="12">
-        <v>2</v>
-      </c>
-      <c r="L50" s="13" t="s">
+      <c r="M50" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N50" s="10">
+        <v>2</v>
+      </c>
+      <c r="O50" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P50" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q50" s="10">
+        <v>2</v>
+      </c>
+      <c r="R50" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M50" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N50" s="10">
-        <v>2</v>
-      </c>
-      <c r="O50" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P50" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q50" s="10">
-        <v>2</v>
-      </c>
-      <c r="R50" s="11" t="s">
-        <v>11</v>
-      </c>
       <c r="S50" s="22" t="s">
         <v>9</v>
       </c>
@@ -4200,23 +4242,23 @@
         <v>2</v>
       </c>
       <c r="U50" s="9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="V50" s="24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="W50" s="8">
         <v>2</v>
       </c>
       <c r="X50" s="9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y50" s="24" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="31"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="14">
         <v>2</v>
       </c>
@@ -4239,35 +4281,35 @@
         <v>2</v>
       </c>
       <c r="I51" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K51" s="12">
+        <v>2</v>
+      </c>
+      <c r="L51" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J51" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K51" s="12">
-        <v>2</v>
-      </c>
-      <c r="L51" s="13" t="s">
+      <c r="M51" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N51" s="10">
+        <v>2</v>
+      </c>
+      <c r="O51" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P51" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q51" s="10">
+        <v>2</v>
+      </c>
+      <c r="R51" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M51" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="N51" s="10">
-        <v>2</v>
-      </c>
-      <c r="O51" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="P51" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q51" s="10">
-        <v>2</v>
-      </c>
-      <c r="R51" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="S51" s="22" t="s">
         <v>4</v>
       </c>
@@ -4275,7 +4317,7 @@
         <v>2</v>
       </c>
       <c r="U51" s="9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="V51" s="24" t="s">
         <v>4</v>
@@ -4284,14 +4326,14 @@
         <v>2</v>
       </c>
       <c r="X51" s="9" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Y51" s="24" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="31"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="14">
         <v>2</v>
       </c>
@@ -4314,64 +4356,1300 @@
         <v>2</v>
       </c>
       <c r="I52" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J52" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K52" s="12">
+        <v>2</v>
+      </c>
+      <c r="L52" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J52" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K52" s="12">
-        <v>2</v>
-      </c>
-      <c r="L52" s="13" t="s">
+      <c r="M52" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N52" s="10">
+        <v>2</v>
+      </c>
+      <c r="O52" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P52" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q52" s="10">
+        <v>2</v>
+      </c>
+      <c r="R52" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M52" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="N52" s="10">
-        <v>2</v>
-      </c>
-      <c r="O52" s="11" t="s">
+      <c r="S52" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="T52" s="8">
+        <v>2</v>
+      </c>
+      <c r="U52" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="V52" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="W52" s="8">
+        <v>2</v>
+      </c>
+      <c r="X52" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y52" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32"/>
+      <c r="L53" s="32"/>
+      <c r="M53" s="32"/>
+      <c r="N53" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="O53" s="32"/>
+      <c r="P53" s="32"/>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="32"/>
+      <c r="S53" s="32"/>
+      <c r="T53" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="U53" s="32"/>
+      <c r="V53" s="32"/>
+      <c r="W53" s="32"/>
+      <c r="X53" s="32"/>
+      <c r="Y53" s="32"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="26">
+        <v>1</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="26">
+        <v>1</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J54" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K54" s="1">
+        <v>1</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M54" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N54" s="3">
+        <v>1</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P54" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>1</v>
+      </c>
+      <c r="R54" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S54" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T54" s="6">
+        <v>1</v>
+      </c>
+      <c r="U54" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V54" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="W54" s="6">
+        <v>1</v>
+      </c>
+      <c r="X54" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y54" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="27"/>
+      <c r="B55" s="26">
+        <v>1</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="26">
+        <v>1</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J55" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K55" s="1">
+        <v>1</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M55" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N55" s="3">
+        <v>1</v>
+      </c>
+      <c r="O55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P55" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q55" s="3">
+        <v>1</v>
+      </c>
+      <c r="R55" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S55" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T55" s="6">
+        <v>1</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V55" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="W55" s="6">
+        <v>1</v>
+      </c>
+      <c r="X55" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y55" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="27"/>
+      <c r="B56" s="26">
+        <v>1</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="26">
+        <v>1</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J56" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K56" s="1">
+        <v>1</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M56" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N56" s="3">
+        <v>1</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P56" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q56" s="3">
+        <v>1</v>
+      </c>
+      <c r="R56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S56" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T56" s="6">
+        <v>1</v>
+      </c>
+      <c r="U56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V56" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="W56" s="6">
+        <v>1</v>
+      </c>
+      <c r="X56" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y56" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="27"/>
+      <c r="B57" s="26">
+        <v>1</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="26">
+        <v>1</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J57" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="1">
+        <v>1</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M57" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N57" s="3">
+        <v>1</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P57" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q57" s="3">
+        <v>1</v>
+      </c>
+      <c r="R57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S57" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="T57" s="6">
+        <v>1</v>
+      </c>
+      <c r="U57" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V57" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="W57" s="6">
+        <v>1</v>
+      </c>
+      <c r="X57" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y57" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="27"/>
+      <c r="B58" s="26">
+        <v>1</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="26">
+        <v>1</v>
+      </c>
+      <c r="F58" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K58" s="1">
+        <v>1</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M58" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N58" s="3">
+        <v>1</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P58" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>1</v>
+      </c>
+      <c r="R58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S58" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="T58" s="6">
+        <v>1</v>
+      </c>
+      <c r="U58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V58" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="W58" s="6">
+        <v>1</v>
+      </c>
+      <c r="X58" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y58" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="27"/>
+      <c r="B59" s="26">
+        <v>1</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="26">
+        <v>1</v>
+      </c>
+      <c r="F59" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K59" s="1">
+        <v>1</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M59" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N59" s="3">
+        <v>1</v>
+      </c>
+      <c r="O59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P59" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q59" s="3">
+        <v>1</v>
+      </c>
+      <c r="R59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S59" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="T59" s="6">
+        <v>1</v>
+      </c>
+      <c r="U59" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V59" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="W59" s="6">
+        <v>1</v>
+      </c>
+      <c r="X59" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y59" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="27"/>
+      <c r="B60" s="26">
+        <v>1</v>
+      </c>
+      <c r="C60" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P52" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q52" s="10">
-        <v>2</v>
-      </c>
-      <c r="R52" s="11" t="s">
+      <c r="D60" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="26">
+        <v>1</v>
+      </c>
+      <c r="F60" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S52" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="T52" s="8">
-        <v>2</v>
-      </c>
-      <c r="U52" s="9" t="s">
+      <c r="G60" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K60" s="1">
+        <v>1</v>
+      </c>
+      <c r="L60" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V52" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="W52" s="8">
-        <v>2</v>
-      </c>
-      <c r="X52" s="9" t="s">
+      <c r="M60" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N60" s="3">
+        <v>1</v>
+      </c>
+      <c r="O60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P60" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q60" s="3">
+        <v>1</v>
+      </c>
+      <c r="R60" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Y52" s="24" t="s">
-        <v>4</v>
+      <c r="S60" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="T60" s="6">
+        <v>1</v>
+      </c>
+      <c r="U60" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="V60" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="W60" s="6">
+        <v>1</v>
+      </c>
+      <c r="X60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y60" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="27"/>
+      <c r="B61" s="26">
+        <v>1</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="26">
+        <v>1</v>
+      </c>
+      <c r="F61" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K61" s="1">
+        <v>1</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M61" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N61" s="3">
+        <v>1</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P61" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q61" s="3">
+        <v>1</v>
+      </c>
+      <c r="R61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S61" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="T61" s="6">
+        <v>1</v>
+      </c>
+      <c r="U61" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="V61" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="W61" s="6">
+        <v>1</v>
+      </c>
+      <c r="X61" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y61" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="27"/>
+      <c r="B62" s="14">
+        <v>2</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="14">
+        <v>2</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="12">
+        <v>2</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J62" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K62" s="12">
+        <v>2</v>
+      </c>
+      <c r="L62" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M62" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N62" s="10">
+        <v>2</v>
+      </c>
+      <c r="O62" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="P62" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q62" s="10">
+        <v>2</v>
+      </c>
+      <c r="R62" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="S62" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="T62" s="8">
+        <v>2</v>
+      </c>
+      <c r="U62" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="V62" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="W62" s="8">
+        <v>2</v>
+      </c>
+      <c r="X62" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y62" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="27"/>
+      <c r="B63" s="14">
+        <v>2</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="14">
+        <v>2</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" s="12">
+        <v>2</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J63" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K63" s="12">
+        <v>2</v>
+      </c>
+      <c r="L63" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M63" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N63" s="10">
+        <v>2</v>
+      </c>
+      <c r="O63" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="P63" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q63" s="10">
+        <v>2</v>
+      </c>
+      <c r="R63" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="S63" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="T63" s="8">
+        <v>2</v>
+      </c>
+      <c r="U63" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="V63" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="W63" s="8">
+        <v>2</v>
+      </c>
+      <c r="X63" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y63" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="27"/>
+      <c r="B64" s="14">
+        <v>2</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="14">
+        <v>2</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" s="12">
+        <v>2</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K64" s="12">
+        <v>2</v>
+      </c>
+      <c r="L64" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M64" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N64" s="10">
+        <v>2</v>
+      </c>
+      <c r="O64" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P64" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q64" s="10">
+        <v>2</v>
+      </c>
+      <c r="R64" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="S64" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="T64" s="8">
+        <v>2</v>
+      </c>
+      <c r="U64" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="V64" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="W64" s="8">
+        <v>2</v>
+      </c>
+      <c r="X64" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y64" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="27"/>
+      <c r="B65" s="14">
+        <v>2</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="14">
+        <v>2</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="12">
+        <v>2</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J65" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K65" s="12">
+        <v>2</v>
+      </c>
+      <c r="L65" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M65" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N65" s="10">
+        <v>2</v>
+      </c>
+      <c r="O65" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P65" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q65" s="10">
+        <v>2</v>
+      </c>
+      <c r="R65" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="S65" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="T65" s="8">
+        <v>2</v>
+      </c>
+      <c r="U65" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="V65" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="W65" s="8">
+        <v>2</v>
+      </c>
+      <c r="X65" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y65" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="27"/>
+      <c r="B66" s="14">
+        <v>2</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="14">
+        <v>2</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" s="12">
+        <v>2</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K66" s="12">
+        <v>2</v>
+      </c>
+      <c r="L66" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M66" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N66" s="10">
+        <v>2</v>
+      </c>
+      <c r="O66" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P66" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q66" s="10">
+        <v>2</v>
+      </c>
+      <c r="R66" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="S66" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="T66" s="8">
+        <v>2</v>
+      </c>
+      <c r="U66" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V66" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="W66" s="8">
+        <v>2</v>
+      </c>
+      <c r="X66" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y66" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="27"/>
+      <c r="B67" s="14">
+        <v>2</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="14">
+        <v>2</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H67" s="12">
+        <v>2</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K67" s="12">
+        <v>2</v>
+      </c>
+      <c r="L67" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M67" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N67" s="10">
+        <v>2</v>
+      </c>
+      <c r="O67" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P67" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q67" s="10">
+        <v>2</v>
+      </c>
+      <c r="R67" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="S67" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="T67" s="8">
+        <v>2</v>
+      </c>
+      <c r="U67" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="V67" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="W67" s="8">
+        <v>2</v>
+      </c>
+      <c r="X67" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y67" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="27"/>
+      <c r="B68" s="14">
+        <v>2</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="14">
+        <v>2</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" s="12">
+        <v>2</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J68" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K68" s="12">
+        <v>2</v>
+      </c>
+      <c r="L68" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M68" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N68" s="10">
+        <v>2</v>
+      </c>
+      <c r="O68" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P68" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q68" s="10">
+        <v>2</v>
+      </c>
+      <c r="R68" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="S68" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="T68" s="8">
+        <v>2</v>
+      </c>
+      <c r="U68" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="V68" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="W68" s="8">
+        <v>2</v>
+      </c>
+      <c r="X68" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y68" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="27"/>
+      <c r="B69" s="14">
+        <v>2</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="14">
+        <v>2</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H69" s="12">
+        <v>2</v>
+      </c>
+      <c r="I69" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J69" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K69" s="12">
+        <v>2</v>
+      </c>
+      <c r="L69" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M69" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N69" s="10">
+        <v>2</v>
+      </c>
+      <c r="O69" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P69" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q69" s="10">
+        <v>2</v>
+      </c>
+      <c r="R69" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="S69" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="T69" s="8">
+        <v>2</v>
+      </c>
+      <c r="U69" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="V69" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="W69" s="8">
+        <v>2</v>
+      </c>
+      <c r="X69" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y69" s="24" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A4:A35"/>
-    <mergeCell ref="A37:A52"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="T2:V2"/>
+  <mergeCells count="23">
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="H53:M53"/>
+    <mergeCell ref="N53:S53"/>
+    <mergeCell ref="T53:Y53"/>
+    <mergeCell ref="A54:A69"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="T1:Y1"/>
@@ -4381,6 +5659,15 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A4:A35"/>
+    <mergeCell ref="A37:A52"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="N36:S36"/>
+    <mergeCell ref="T36:Y36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
print long format so I can fit it with ALANN
</commit_message>
<xml_diff>
--- a/design/sets.xlsx
+++ b/design/sets.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/santiago_castiellodeobeso_yale_edu/Documents/Collaborations/Brooklyn_College/categoricalReversalLerning/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D3FDCAC-F565-494C-B6AE-99B71A65B74B}"/>
+  <xr:revisionPtr revIDLastSave="413" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC346144-CA76-407D-9F6E-445B00C7E265}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="table1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="57">
   <si>
     <t>phase</t>
   </si>
@@ -136,12 +137,104 @@
   <si>
     <t>Set8</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Reversal</t>
+  </si>
+  <si>
+    <t>Category Total Reversal</t>
+  </si>
+  <si>
+    <t>Category Partial Reversal</t>
+  </si>
+  <si>
+    <t>→N</t>
+  </si>
+  <si>
+    <t>S←</t>
+  </si>
+  <si>
+    <t>Table 1.</t>
+  </si>
+  <si>
+    <t>Cues</t>
+  </si>
+  <si>
+    <t>Cat.</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>non-reversal</t>
+  </si>
+  <si>
+    <t>reversal</t>
+  </si>
+  <si>
+    <t>Categorical Reversal Learning Experimental Design (hard)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Easy version is not presented. A, B, C, D, E, F, G, and H are cues in form of fractals; S← and →N are two distinct categories (Cat.).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +265,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,8 +335,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -237,11 +350,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -287,6 +418,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -296,15 +440,28 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="E9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="T69" sqref="T69"/>
     </sheetView>
   </sheetViews>
@@ -620,80 +777,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="28" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="29" t="s">
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
     </row>
     <row r="2" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31" t="s">
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31" t="s">
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="28" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="29" t="s">
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29" t="s">
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="14" t="s">
@@ -770,7 +927,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="32" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="26">
@@ -847,7 +1004,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="27"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="26">
         <v>1</v>
       </c>
@@ -922,7 +1079,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="27"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="26">
         <v>1</v>
       </c>
@@ -997,7 +1154,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="27"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="26">
         <v>1</v>
       </c>
@@ -1072,7 +1229,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="27"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="26">
         <v>1</v>
       </c>
@@ -1147,7 +1304,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="27"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="26">
         <v>1</v>
       </c>
@@ -1222,7 +1379,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="27"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="26">
         <v>1</v>
       </c>
@@ -1297,7 +1454,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="27"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="26">
         <v>1</v>
       </c>
@@ -1372,7 +1529,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="27"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="26">
         <v>1</v>
       </c>
@@ -1447,7 +1604,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="27"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="26">
         <v>1</v>
       </c>
@@ -1522,7 +1679,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="27"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="26">
         <v>1</v>
       </c>
@@ -1597,7 +1754,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="27"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="26">
         <v>1</v>
       </c>
@@ -1672,7 +1829,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="27"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="26">
         <v>1</v>
       </c>
@@ -1747,7 +1904,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="27"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="26">
         <v>1</v>
       </c>
@@ -1822,7 +1979,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="27"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="26">
         <v>1</v>
       </c>
@@ -1897,7 +2054,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="27"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="26">
         <v>1</v>
       </c>
@@ -1972,7 +2129,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="27"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="14">
         <v>2</v>
       </c>
@@ -2047,7 +2204,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="27"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="14">
         <v>2</v>
       </c>
@@ -2122,7 +2279,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="27"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="14">
         <v>2</v>
       </c>
@@ -2197,7 +2354,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="27"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="14">
         <v>2</v>
       </c>
@@ -2272,7 +2429,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="27"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="14">
         <v>2</v>
       </c>
@@ -2347,7 +2504,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="27"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="14">
         <v>2</v>
       </c>
@@ -2422,7 +2579,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="27"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="14">
         <v>2</v>
       </c>
@@ -2497,7 +2654,7 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="27"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="14">
         <v>2</v>
       </c>
@@ -2572,7 +2729,7 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="27"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="14">
         <v>2</v>
       </c>
@@ -2647,7 +2804,7 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="27"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="14">
         <v>2</v>
       </c>
@@ -2722,7 +2879,7 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="27"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="14">
         <v>2</v>
       </c>
@@ -2797,7 +2954,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="27"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="14">
         <v>2</v>
       </c>
@@ -2872,7 +3029,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="27"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -2947,7 +3104,7 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="27"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="14">
         <v>2</v>
       </c>
@@ -3022,7 +3179,7 @@
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="27"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -3097,7 +3254,7 @@
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="27"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="14">
         <v>2</v>
       </c>
@@ -3172,41 +3329,41 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32" t="s">
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32" t="s">
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="32"/>
-      <c r="R36" s="32"/>
-      <c r="S36" s="32"/>
-      <c r="T36" s="32" t="s">
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="32"/>
-      <c r="X36" s="32"/>
-      <c r="Y36" s="32"/>
+      <c r="U36" s="35"/>
+      <c r="V36" s="35"/>
+      <c r="W36" s="35"/>
+      <c r="X36" s="35"/>
+      <c r="Y36" s="35"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="32" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="26">
@@ -3283,7 +3440,7 @@
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="27"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="26">
         <v>1</v>
       </c>
@@ -3358,7 +3515,7 @@
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="27"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="26">
         <v>1</v>
       </c>
@@ -3433,7 +3590,7 @@
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="27"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="26">
         <v>1</v>
       </c>
@@ -3508,7 +3665,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="27"/>
+      <c r="A41" s="32"/>
       <c r="B41" s="26">
         <v>1</v>
       </c>
@@ -3583,7 +3740,7 @@
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="27"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="26">
         <v>1</v>
       </c>
@@ -3658,7 +3815,7 @@
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="27"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="26">
         <v>1</v>
       </c>
@@ -3733,7 +3890,7 @@
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="27"/>
+      <c r="A44" s="32"/>
       <c r="B44" s="26">
         <v>1</v>
       </c>
@@ -3808,7 +3965,7 @@
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="27"/>
+      <c r="A45" s="32"/>
       <c r="B45" s="14">
         <v>2</v>
       </c>
@@ -3883,7 +4040,7 @@
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="27"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="14">
         <v>2</v>
       </c>
@@ -3958,7 +4115,7 @@
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="27"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="14">
         <v>2</v>
       </c>
@@ -4033,7 +4190,7 @@
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="27"/>
+      <c r="A48" s="32"/>
       <c r="B48" s="14">
         <v>2</v>
       </c>
@@ -4108,7 +4265,7 @@
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="27"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="14">
         <v>2</v>
       </c>
@@ -4183,7 +4340,7 @@
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="27"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="14">
         <v>2</v>
       </c>
@@ -4258,7 +4415,7 @@
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="27"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="14">
         <v>2</v>
       </c>
@@ -4333,7 +4490,7 @@
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="27"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="14">
         <v>2</v>
       </c>
@@ -4408,41 +4565,41 @@
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="32" t="s">
+      <c r="B53" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32" t="s">
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-      <c r="M53" s="32"/>
-      <c r="N53" s="32" t="s">
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="O53" s="32"/>
-      <c r="P53" s="32"/>
-      <c r="Q53" s="32"/>
-      <c r="R53" s="32"/>
-      <c r="S53" s="32"/>
-      <c r="T53" s="32" t="s">
+      <c r="O53" s="35"/>
+      <c r="P53" s="35"/>
+      <c r="Q53" s="35"/>
+      <c r="R53" s="35"/>
+      <c r="S53" s="35"/>
+      <c r="T53" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="U53" s="32"/>
-      <c r="V53" s="32"/>
-      <c r="W53" s="32"/>
-      <c r="X53" s="32"/>
-      <c r="Y53" s="32"/>
+      <c r="U53" s="35"/>
+      <c r="V53" s="35"/>
+      <c r="W53" s="35"/>
+      <c r="X53" s="35"/>
+      <c r="Y53" s="35"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="32" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="26">
@@ -4519,7 +4676,7 @@
       </c>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="27"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="26">
         <v>1</v>
       </c>
@@ -4594,7 +4751,7 @@
       </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="27"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="26">
         <v>1</v>
       </c>
@@ -4669,7 +4826,7 @@
       </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="27"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="26">
         <v>1</v>
       </c>
@@ -4744,7 +4901,7 @@
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="27"/>
+      <c r="A58" s="32"/>
       <c r="B58" s="26">
         <v>1</v>
       </c>
@@ -4819,7 +4976,7 @@
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="27"/>
+      <c r="A59" s="32"/>
       <c r="B59" s="26">
         <v>1</v>
       </c>
@@ -4894,7 +5051,7 @@
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="27"/>
+      <c r="A60" s="32"/>
       <c r="B60" s="26">
         <v>1</v>
       </c>
@@ -4969,7 +5126,7 @@
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="27"/>
+      <c r="A61" s="32"/>
       <c r="B61" s="26">
         <v>1</v>
       </c>
@@ -5044,7 +5201,7 @@
       </c>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="27"/>
+      <c r="A62" s="32"/>
       <c r="B62" s="14">
         <v>2</v>
       </c>
@@ -5119,7 +5276,7 @@
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="27"/>
+      <c r="A63" s="32"/>
       <c r="B63" s="14">
         <v>2</v>
       </c>
@@ -5194,7 +5351,7 @@
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="27"/>
+      <c r="A64" s="32"/>
       <c r="B64" s="14">
         <v>2</v>
       </c>
@@ -5269,7 +5426,7 @@
       </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="27"/>
+      <c r="A65" s="32"/>
       <c r="B65" s="14">
         <v>2</v>
       </c>
@@ -5344,7 +5501,7 @@
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="27"/>
+      <c r="A66" s="32"/>
       <c r="B66" s="14">
         <v>2</v>
       </c>
@@ -5419,7 +5576,7 @@
       </c>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="27"/>
+      <c r="A67" s="32"/>
       <c r="B67" s="14">
         <v>2</v>
       </c>
@@ -5494,7 +5651,7 @@
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="27"/>
+      <c r="A68" s="32"/>
       <c r="B68" s="14">
         <v>2</v>
       </c>
@@ -5569,7 +5726,7 @@
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="27"/>
+      <c r="A69" s="32"/>
       <c r="B69" s="14">
         <v>2</v>
       </c>
@@ -5650,7 +5807,6 @@
     <mergeCell ref="N53:S53"/>
     <mergeCell ref="T53:Y53"/>
     <mergeCell ref="A54:A69"/>
-    <mergeCell ref="W2:Y2"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="B2:D2"/>
@@ -5668,8 +5824,412 @@
     <mergeCell ref="H36:M36"/>
     <mergeCell ref="N36:S36"/>
     <mergeCell ref="T36:Y36"/>
+    <mergeCell ref="W2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0E5C93-11B3-4D1D-A76B-B4C888F80A08}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="3.3671875" customWidth="1"/>
+    <col min="6" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="11.5234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="39"/>
+      <c r="J4" s="27"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="39"/>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
waiting for andy's response email
</commit_message>
<xml_diff>
--- a/design/sets.xlsx
+++ b/design/sets.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="413" documentId="11_F25DC773A252ABDACC10482A911958D25BDE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC346144-CA76-407D-9F6E-445B00C7E265}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,6 +431,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -461,7 +462,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,115 +744,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView topLeftCell="E9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T69" sqref="T69"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.7890625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.3671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.76171875" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.3515625" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:25" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="33" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="34" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-    </row>
-    <row r="2" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="B2" s="36" t="s">
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+    </row>
+    <row r="2" spans="1:25" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="B2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37" t="s">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="33" t="s">
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33" t="s">
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="34" t="s">
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34" t="s">
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.5">
       <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
@@ -926,8 +926,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A4" s="33" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="26">
@@ -1003,8 +1003,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="32"/>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A5" s="33"/>
       <c r="B5" s="26">
         <v>1</v>
       </c>
@@ -1078,8 +1078,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="32"/>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A6" s="33"/>
       <c r="B6" s="26">
         <v>1</v>
       </c>
@@ -1153,8 +1153,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="32"/>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A7" s="33"/>
       <c r="B7" s="26">
         <v>1</v>
       </c>
@@ -1228,8 +1228,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="32"/>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A8" s="33"/>
       <c r="B8" s="26">
         <v>1</v>
       </c>
@@ -1303,8 +1303,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="32"/>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A9" s="33"/>
       <c r="B9" s="26">
         <v>1</v>
       </c>
@@ -1378,8 +1378,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="32"/>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A10" s="33"/>
       <c r="B10" s="26">
         <v>1</v>
       </c>
@@ -1453,8 +1453,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="32"/>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A11" s="33"/>
       <c r="B11" s="26">
         <v>1</v>
       </c>
@@ -1528,8 +1528,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A12" s="33"/>
       <c r="B12" s="26">
         <v>1</v>
       </c>
@@ -1603,8 +1603,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="32"/>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A13" s="33"/>
       <c r="B13" s="26">
         <v>1</v>
       </c>
@@ -1678,8 +1678,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="32"/>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A14" s="33"/>
       <c r="B14" s="26">
         <v>1</v>
       </c>
@@ -1753,8 +1753,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="32"/>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A15" s="33"/>
       <c r="B15" s="26">
         <v>1</v>
       </c>
@@ -1828,8 +1828,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="32"/>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A16" s="33"/>
       <c r="B16" s="26">
         <v>1</v>
       </c>
@@ -1903,8 +1903,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="32"/>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A17" s="33"/>
       <c r="B17" s="26">
         <v>1</v>
       </c>
@@ -1978,8 +1978,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="32"/>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A18" s="33"/>
       <c r="B18" s="26">
         <v>1</v>
       </c>
@@ -2053,8 +2053,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="32"/>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A19" s="33"/>
       <c r="B19" s="26">
         <v>1</v>
       </c>
@@ -2128,8 +2128,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="32"/>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A20" s="33"/>
       <c r="B20" s="14">
         <v>2</v>
       </c>
@@ -2203,8 +2203,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="32"/>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A21" s="33"/>
       <c r="B21" s="14">
         <v>2</v>
       </c>
@@ -2278,8 +2278,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="32"/>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A22" s="33"/>
       <c r="B22" s="14">
         <v>2</v>
       </c>
@@ -2353,8 +2353,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="32"/>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A23" s="33"/>
       <c r="B23" s="14">
         <v>2</v>
       </c>
@@ -2428,8 +2428,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="32"/>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A24" s="33"/>
       <c r="B24" s="14">
         <v>2</v>
       </c>
@@ -2503,8 +2503,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="32"/>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A25" s="33"/>
       <c r="B25" s="14">
         <v>2</v>
       </c>
@@ -2578,8 +2578,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="32"/>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A26" s="33"/>
       <c r="B26" s="14">
         <v>2</v>
       </c>
@@ -2653,8 +2653,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="32"/>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A27" s="33"/>
       <c r="B27" s="14">
         <v>2</v>
       </c>
@@ -2728,8 +2728,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="32"/>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A28" s="33"/>
       <c r="B28" s="14">
         <v>2</v>
       </c>
@@ -2803,8 +2803,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="32"/>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A29" s="33"/>
       <c r="B29" s="14">
         <v>2</v>
       </c>
@@ -2878,8 +2878,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="32"/>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A30" s="33"/>
       <c r="B30" s="14">
         <v>2</v>
       </c>
@@ -2953,8 +2953,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="32"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A31" s="33"/>
       <c r="B31" s="14">
         <v>2</v>
       </c>
@@ -3028,8 +3028,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="32"/>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A32" s="33"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -3103,8 +3103,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A33" s="33"/>
       <c r="B33" s="14">
         <v>2</v>
       </c>
@@ -3178,8 +3178,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="32"/>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A34" s="33"/>
       <c r="B34" s="14">
         <v>2</v>
       </c>
@@ -3253,8 +3253,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="32"/>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A35" s="33"/>
       <c r="B35" s="14">
         <v>2</v>
       </c>
@@ -3328,42 +3328,42 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="35" t="s">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="B36" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35" t="s">
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35" t="s">
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="35"/>
-      <c r="S36" s="35"/>
-      <c r="T36" s="35" t="s">
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="U36" s="35"/>
-      <c r="V36" s="35"/>
-      <c r="W36" s="35"/>
-      <c r="X36" s="35"/>
-      <c r="Y36" s="35"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="32" t="s">
+      <c r="U36" s="36"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="36"/>
+      <c r="X36" s="36"/>
+      <c r="Y36" s="36"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A37" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="26">
@@ -3439,8 +3439,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="32"/>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A38" s="33"/>
       <c r="B38" s="26">
         <v>1</v>
       </c>
@@ -3514,8 +3514,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="32"/>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A39" s="33"/>
       <c r="B39" s="26">
         <v>1</v>
       </c>
@@ -3589,8 +3589,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="32"/>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A40" s="33"/>
       <c r="B40" s="26">
         <v>1</v>
       </c>
@@ -3664,8 +3664,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="32"/>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A41" s="33"/>
       <c r="B41" s="26">
         <v>1</v>
       </c>
@@ -3739,8 +3739,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="32"/>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A42" s="33"/>
       <c r="B42" s="26">
         <v>1</v>
       </c>
@@ -3814,8 +3814,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="32"/>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A43" s="33"/>
       <c r="B43" s="26">
         <v>1</v>
       </c>
@@ -3889,8 +3889,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="32"/>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A44" s="33"/>
       <c r="B44" s="26">
         <v>1</v>
       </c>
@@ -3964,8 +3964,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="32"/>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A45" s="33"/>
       <c r="B45" s="14">
         <v>2</v>
       </c>
@@ -4039,8 +4039,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="32"/>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A46" s="33"/>
       <c r="B46" s="14">
         <v>2</v>
       </c>
@@ -4114,8 +4114,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="32"/>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A47" s="33"/>
       <c r="B47" s="14">
         <v>2</v>
       </c>
@@ -4189,8 +4189,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="32"/>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A48" s="33"/>
       <c r="B48" s="14">
         <v>2</v>
       </c>
@@ -4264,8 +4264,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="32"/>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A49" s="33"/>
       <c r="B49" s="14">
         <v>2</v>
       </c>
@@ -4339,8 +4339,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="32"/>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A50" s="33"/>
       <c r="B50" s="14">
         <v>2</v>
       </c>
@@ -4414,8 +4414,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="32"/>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A51" s="33"/>
       <c r="B51" s="14">
         <v>2</v>
       </c>
@@ -4489,8 +4489,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="32"/>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A52" s="33"/>
       <c r="B52" s="14">
         <v>2</v>
       </c>
@@ -4564,42 +4564,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" s="35" t="s">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="B53" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35" t="s">
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35" t="s">
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="36"/>
+      <c r="N53" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="O53" s="35"/>
-      <c r="P53" s="35"/>
-      <c r="Q53" s="35"/>
-      <c r="R53" s="35"/>
-      <c r="S53" s="35"/>
-      <c r="T53" s="35" t="s">
+      <c r="O53" s="36"/>
+      <c r="P53" s="36"/>
+      <c r="Q53" s="36"/>
+      <c r="R53" s="36"/>
+      <c r="S53" s="36"/>
+      <c r="T53" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="U53" s="35"/>
-      <c r="V53" s="35"/>
-      <c r="W53" s="35"/>
-      <c r="X53" s="35"/>
-      <c r="Y53" s="35"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="32" t="s">
+      <c r="U53" s="36"/>
+      <c r="V53" s="36"/>
+      <c r="W53" s="36"/>
+      <c r="X53" s="36"/>
+      <c r="Y53" s="36"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A54" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="26">
@@ -4675,8 +4675,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="32"/>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A55" s="33"/>
       <c r="B55" s="26">
         <v>1</v>
       </c>
@@ -4750,8 +4750,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="32"/>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A56" s="33"/>
       <c r="B56" s="26">
         <v>1</v>
       </c>
@@ -4825,8 +4825,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="32"/>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A57" s="33"/>
       <c r="B57" s="26">
         <v>1</v>
       </c>
@@ -4900,8 +4900,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="32"/>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A58" s="33"/>
       <c r="B58" s="26">
         <v>1</v>
       </c>
@@ -4975,8 +4975,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="32"/>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A59" s="33"/>
       <c r="B59" s="26">
         <v>1</v>
       </c>
@@ -5050,8 +5050,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A60" s="33"/>
       <c r="B60" s="26">
         <v>1</v>
       </c>
@@ -5125,8 +5125,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="32"/>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A61" s="33"/>
       <c r="B61" s="26">
         <v>1</v>
       </c>
@@ -5200,8 +5200,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="32"/>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A62" s="33"/>
       <c r="B62" s="14">
         <v>2</v>
       </c>
@@ -5275,8 +5275,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="32"/>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A63" s="33"/>
       <c r="B63" s="14">
         <v>2</v>
       </c>
@@ -5350,8 +5350,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="32"/>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A64" s="33"/>
       <c r="B64" s="14">
         <v>2</v>
       </c>
@@ -5425,8 +5425,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="32"/>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A65" s="33"/>
       <c r="B65" s="14">
         <v>2</v>
       </c>
@@ -5500,8 +5500,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="32"/>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A66" s="33"/>
       <c r="B66" s="14">
         <v>2</v>
       </c>
@@ -5575,8 +5575,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="32"/>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A67" s="33"/>
       <c r="B67" s="14">
         <v>2</v>
       </c>
@@ -5650,8 +5650,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="32"/>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A68" s="33"/>
       <c r="B68" s="14">
         <v>2</v>
       </c>
@@ -5725,8 +5725,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="32"/>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.5">
+      <c r="A69" s="33"/>
       <c r="B69" s="14">
         <v>2</v>
       </c>
@@ -5835,20 +5835,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0E5C93-11B3-4D1D-A76B-B4C888F80A08}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="3.3671875" customWidth="1"/>
+    <col min="5" max="5" width="3.3515625" customWidth="1"/>
     <col min="6" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="11.5234375" customWidth="1"/>
+    <col min="10" max="10" width="11.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A1" s="32" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="27"/>
@@ -5861,77 +5861,77 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A2" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="41" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A3" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="39" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A4" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="28"/>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="40"/>
       <c r="J4" s="27"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A5" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="28"/>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39" t="s">
+      <c r="G5" s="40"/>
+      <c r="H5" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="27"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6" s="29" t="s">
         <v>50</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" s="28" t="s">
         <v>33</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" s="28" t="s">
         <v>34</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" s="28" t="s">
         <v>35</v>
       </c>
@@ -6051,7 +6051,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" s="28" t="s">
         <v>36</v>
       </c>
@@ -6081,7 +6081,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" s="28" t="s">
         <v>37</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" s="28" t="s">
         <v>38</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" s="28" t="s">
         <v>39</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A14" s="29" t="s">
         <v>40</v>
       </c>
@@ -6201,19 +6201,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>